<commit_message>
Added 2 graphs to the Spreadsheet(48 cities)
</commit_message>
<xml_diff>
--- a/Result_sheet.xlsx
+++ b/Result_sheet.xlsx
@@ -362,7 +362,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="13">
   <si>
     <t>48 CITIES</t>
   </si>
@@ -451,12 +451,15 @@
       <t xml:space="preserve"> Simulated Annealing</t>
     </r>
   </si>
+  <si>
+    <t>Average</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,6 +524,14 @@
     <font>
       <b/>
       <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -613,7 +624,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="3"/>
@@ -639,6 +650,10 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
@@ -660,136 +675,2898 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Line</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Graph showing fitness for the 4 different Algorithms for 48 cities </a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Simulated Annealing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>('48'!$D$53,'48'!$G$53,'48'!$J$53,'48'!$M$53,'48'!$P$53,'48'!$S$53,'48'!$V$53,'48'!$Y$53,'48'!$AB$53,'48'!$AE$53)</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('48'!$C$65,'48'!$F$65,'48'!$I$65,'48'!$L$65,'48'!$O$65,'48'!$R$65,'48'!$U$65,'48'!$X$65,'48'!$AA$65,'48'!$AD$65)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>40740.680117002281</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42495.550132819422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42371.756863898794</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39534.564988198043</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>39193.875388758395</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38023.602570881136</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>38458.926283995483</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39066.91620513508</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37502.696591863489</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36552.108284463764</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-37C0-4E80-930F-55AEF12F931D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Stochastic Hill Climbing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>('48'!$C$49,'48'!$F$49,'48'!$I$49,'48'!$L$49,'48'!$O$49,'48'!$R$49,'48'!$U$49,'48'!$X$49,'48'!$AA$49,'48'!$AD$49)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>47680.164899101728</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44837.436550754748</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44339.844799522005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43439.582744091036</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44402.643189703471</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43768.613270000955</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44896.538901347478</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44642.470277928034</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45015.386576053352</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45005.592412111029</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-37C0-4E80-930F-55AEF12F931D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Random Restart Hill Climbing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>('48'!$C$33,'48'!$F$33,'48'!$I$33,'48'!$L$33,'48'!$O$33,'48'!$R$33,'48'!$U$33,'48'!$X$33,'48'!$AA$33,'48'!$AD$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>45949.797477521897</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46675.488346668302</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44212.860590590746</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44676.062213810263</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43928.29929568238</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43860.212419729229</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45214.886952463465</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45646.430732534158</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45314.593443100501</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>44889.323928779813</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-37C0-4E80-930F-55AEF12F931D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Random Mutation Hill Climbing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>('48'!$C$17,'48'!$F$17,'48'!$I$17,'48'!$L$17,'48'!$O$17,'48'!$R$17,'48'!$U$17,'48'!$X$17,'48'!$AA$17,'48'!$AD$17)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>48604.81815781496</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>47359.561565574943</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47692.670660948803</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47755.911010290234</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>46673.873574000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50051.412713514968</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>47870.426988658422</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46487.498944668492</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47303.808572816313</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46179.717035531285</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-37C0-4E80-930F-55AEF12F931D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="684880752"/>
+        <c:axId val="693062640"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="684880752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of Iterations</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                    <a:alpha val="99000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="693062640"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="693062640"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="51000"/>
+          <c:min val="35000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Average Fitness</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="684880752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Line Graph showing</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> Efficiency against Optimal Tour for 4 different Algorthms for 48 Cities</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Simulated Annealing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>('48'!$D$53,'48'!$G$53,'48'!$J$53,'48'!$M$53,'48'!$P$53,'48'!$S$53,'48'!$V$53,'48'!$Y$53,'48'!$AB$53,'48'!$AE$53)</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('48'!$D$65,'48'!$G$65,'48'!$J$65,'48'!$M$65,'48'!$P$65,'48'!$S$65,'48'!$V$65,'48'!$Y$65,'48'!$AB$65,'48'!$AE$65)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>82.522000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>79.673000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>79.460000000000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>84.830999999999989</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>85.763000000000005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>88.277000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>85.991</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>89.47799999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91.788000000000011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-AFC9-48A1-92C4-BF342A0AE096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Stochastic Hill Climbing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>('48'!$D$49,'48'!$G$49,'48'!$J$49,'48'!$M$49,'48'!$P$49,'48'!$S$49,'48'!$V$49,'48'!$Y$49,'48'!$AB$49,'48'!$AE$49)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>70.60799999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>75.147000000000006</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75.771000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>77.379000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76.064999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76.948999999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>75.018000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75.298000000000016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74.96899999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>74.751000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-AFC9-48A1-92C4-BF342A0AE096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Random Restart Hill Climbing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>('48'!$D$33,'48'!$G$33,'48'!$J$33,'48'!$M$33,'48'!$P$33,'48'!$S$33,'48'!$V$33,'48'!$Y$33,'48'!$AB$33,'48'!$AE$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>73.371000000000009</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.174999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>76.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75.289999999999992</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>76.514999999999986</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77.415999999999997</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>74.456999999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>73.620999999999995</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>74.108999999999995</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>74.89200000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-AFC9-48A1-92C4-BF342A0AE096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Random Mutation Hill Climbing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>('48'!$D$17,'48'!$G$17,'48'!$J$17,'48'!$M$17,'48'!$P$17,'48'!$S$17,'48'!$V$17,'48'!$Y$17,'48'!$AB$17,'48'!$AE$17)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>69.277000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>71.546999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70.747</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.712999999999994</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>72.14500000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67.166000000000011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71.042000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72.292999999999978</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>71.097999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>73.269000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-AFC9-48A1-92C4-BF342A0AE096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="847628016"/>
+        <c:axId val="853267280"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="847628016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> of Iterations</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="853267280"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="853267280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+          <c:min val="60"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Average Efficiecny</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="847628016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>32658</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>44753</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>270934</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>33866</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{503FA7D1-57FE-4638-BD96-B4A021307AD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>440266</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>541865</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66597250-939C-4B73-BE63-97AF893CAA0E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_40000" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_80000" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_90000" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_10000" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_20000" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_20000" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_70000" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_50000" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_70000" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_80000" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_60001" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_20000" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_10000" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_60000" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_10000" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_100000" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_40000" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_100000" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_10000" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_70000" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_60000" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_30000" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_80000" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_70000" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_50000" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_60000" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_90000" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_90000" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_40000" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_100000" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_30000" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_80000" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_60000" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_50000" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_40000" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_30000" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_20000" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_10000" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_100000" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_90000" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_90000" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_80000" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_70000" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_60001" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_60000" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_40000" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_30000" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_20000" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_10000" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_100000" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_80000" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_90000" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_80000" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_70000" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_60000" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_70000" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_60000" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_50000" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_40000" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_30000" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_20000" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1089,10 +3866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL64"/>
+  <dimension ref="A1:AL65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD68" sqref="AD68:AF71"/>
+    <sheetView tabSelected="1" topLeftCell="F43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Z99" sqref="Z99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2328,6 +5105,131 @@
         <v>52.94</v>
       </c>
     </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B17" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="12">
+        <f>AVERAGE(C7:C16)</f>
+        <v>48604.81815781496</v>
+      </c>
+      <c r="D17" s="12">
+        <f>AVERAGE(D7:D16)</f>
+        <v>69.277000000000001</v>
+      </c>
+      <c r="E17" s="12">
+        <f>AVERAGE(E7:E16)</f>
+        <v>57.125000000000014</v>
+      </c>
+      <c r="F17" s="12">
+        <f>AVERAGE(F7:F16)</f>
+        <v>47359.561565574943</v>
+      </c>
+      <c r="G17" s="12">
+        <f>AVERAGE(G7:G16)</f>
+        <v>71.546999999999997</v>
+      </c>
+      <c r="H17" s="12">
+        <f>AVERAGE(H7:H16)</f>
+        <v>58.999000000000002</v>
+      </c>
+      <c r="I17" s="12">
+        <f>AVERAGE(I7:I16)</f>
+        <v>47692.670660948803</v>
+      </c>
+      <c r="J17" s="12">
+        <f>AVERAGE(J7:J16)</f>
+        <v>70.747</v>
+      </c>
+      <c r="K17" s="12">
+        <f>AVERAGE(K7:K16)</f>
+        <v>58.338000000000001</v>
+      </c>
+      <c r="L17" s="12">
+        <f>AVERAGE(L7:L16)</f>
+        <v>47755.911010290234</v>
+      </c>
+      <c r="M17" s="12">
+        <f>AVERAGE(M7:M16)</f>
+        <v>70.712999999999994</v>
+      </c>
+      <c r="N17" s="12">
+        <f>AVERAGE(N7:N16)</f>
+        <v>58.311000000000014</v>
+      </c>
+      <c r="O17" s="12">
+        <f>AVERAGE(O7:O16)</f>
+        <v>46673.873574000005</v>
+      </c>
+      <c r="P17" s="12">
+        <f>AVERAGE(P7:P16)</f>
+        <v>72.14500000000001</v>
+      </c>
+      <c r="Q17" s="12">
+        <f>AVERAGE(Q7:Q16)</f>
+        <v>59.491</v>
+      </c>
+      <c r="R17" s="12">
+        <f>AVERAGE(R7:R16)</f>
+        <v>50051.412713514968</v>
+      </c>
+      <c r="S17" s="12">
+        <f>AVERAGE(S7:S16)</f>
+        <v>67.166000000000011</v>
+      </c>
+      <c r="T17" s="12">
+        <f>AVERAGE(T7:T16)</f>
+        <v>55.386000000000003</v>
+      </c>
+      <c r="U17" s="12">
+        <f>AVERAGE(U7:U16)</f>
+        <v>47870.426988658422</v>
+      </c>
+      <c r="V17" s="12">
+        <f>AVERAGE(V7:V16)</f>
+        <v>71.042000000000002</v>
+      </c>
+      <c r="W17" s="12">
+        <f>AVERAGE(W7:W16)</f>
+        <v>58.580999999999996</v>
+      </c>
+      <c r="X17" s="12">
+        <f>AVERAGE(X7:X16)</f>
+        <v>46487.498944668492</v>
+      </c>
+      <c r="Y17" s="12">
+        <f>AVERAGE(Y7:Y16)</f>
+        <v>72.292999999999978</v>
+      </c>
+      <c r="Z17" s="12">
+        <f>AVERAGE(Z7:Z16)</f>
+        <v>59.613999999999997</v>
+      </c>
+      <c r="AA17" s="12">
+        <f>AVERAGE(AA7:AA16)</f>
+        <v>47303.808572816313</v>
+      </c>
+      <c r="AB17" s="12">
+        <f>AVERAGE(AB7:AB16)</f>
+        <v>71.097999999999999</v>
+      </c>
+      <c r="AC17" s="12">
+        <f>AVERAGE(AC7:AC16)</f>
+        <v>58.628</v>
+      </c>
+      <c r="AD17" s="12">
+        <f>AVERAGE(AD7:AD16)</f>
+        <v>46179.717035531285</v>
+      </c>
+      <c r="AE17" s="12">
+        <f>AVERAGE(AE7:AE16)</f>
+        <v>73.269000000000005</v>
+      </c>
+      <c r="AF17" s="12">
+        <f>AVERAGE(AF7:AF16)</f>
+        <v>60.42</v>
+      </c>
+    </row>
     <row r="19" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
@@ -3470,6 +6372,131 @@
         <v>61.64</v>
       </c>
     </row>
+    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B33" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="12">
+        <f>AVERAGE(C23:C32)</f>
+        <v>45949.797477521897</v>
+      </c>
+      <c r="D33" s="12">
+        <f>AVERAGE(D23:D32)</f>
+        <v>73.371000000000009</v>
+      </c>
+      <c r="E33" s="12">
+        <f>AVERAGE(E23:E32)</f>
+        <v>60.501999999999995</v>
+      </c>
+      <c r="F33" s="12">
+        <f>AVERAGE(F23:F32)</f>
+        <v>46675.488346668302</v>
+      </c>
+      <c r="G33" s="12">
+        <f>AVERAGE(G23:G32)</f>
+        <v>72.174999999999997</v>
+      </c>
+      <c r="H33" s="12">
+        <f>AVERAGE(H23:H32)</f>
+        <v>59.518000000000008</v>
+      </c>
+      <c r="I33" s="12">
+        <f>AVERAGE(I23:I32)</f>
+        <v>44212.860590590746</v>
+      </c>
+      <c r="J33" s="12">
+        <f>AVERAGE(J23:J32)</f>
+        <v>76.09</v>
+      </c>
+      <c r="K33" s="12">
+        <f>AVERAGE(K23:K32)</f>
+        <v>62.744000000000007</v>
+      </c>
+      <c r="L33" s="12">
+        <f>AVERAGE(L23:L32)</f>
+        <v>44676.062213810263</v>
+      </c>
+      <c r="M33" s="12">
+        <f>AVERAGE(M23:M32)</f>
+        <v>75.289999999999992</v>
+      </c>
+      <c r="N33" s="12">
+        <f>AVERAGE(N23:N32)</f>
+        <v>62.084000000000003</v>
+      </c>
+      <c r="O33" s="12">
+        <f>AVERAGE(O23:O32)</f>
+        <v>43928.29929568238</v>
+      </c>
+      <c r="P33" s="12">
+        <f>AVERAGE(P23:P32)</f>
+        <v>76.514999999999986</v>
+      </c>
+      <c r="Q33" s="12">
+        <f>AVERAGE(Q23:Q32)</f>
+        <v>63.092999999999996</v>
+      </c>
+      <c r="R33" s="12">
+        <f>AVERAGE(R23:R32)</f>
+        <v>43860.212419729229</v>
+      </c>
+      <c r="S33" s="12">
+        <f>AVERAGE(S23:S32)</f>
+        <v>77.415999999999997</v>
+      </c>
+      <c r="T33" s="12">
+        <f>AVERAGE(T23:T32)</f>
+        <v>63.840000000000011</v>
+      </c>
+      <c r="U33" s="12">
+        <f>AVERAGE(U23:U32)</f>
+        <v>45214.886952463465</v>
+      </c>
+      <c r="V33" s="12">
+        <f>AVERAGE(V23:V32)</f>
+        <v>74.456999999999994</v>
+      </c>
+      <c r="W33" s="12">
+        <f>AVERAGE(W23:W32)</f>
+        <v>61.396999999999991</v>
+      </c>
+      <c r="X33" s="12">
+        <f>AVERAGE(X23:X32)</f>
+        <v>45646.430732534158</v>
+      </c>
+      <c r="Y33" s="12">
+        <f>AVERAGE(Y23:Y32)</f>
+        <v>73.620999999999995</v>
+      </c>
+      <c r="Z33" s="12">
+        <f>AVERAGE(Z23:Z32)</f>
+        <v>60.71</v>
+      </c>
+      <c r="AA33" s="12">
+        <f>AVERAGE(AA23:AA32)</f>
+        <v>45314.593443100501</v>
+      </c>
+      <c r="AB33" s="12">
+        <f>AVERAGE(AB23:AB32)</f>
+        <v>74.108999999999995</v>
+      </c>
+      <c r="AC33" s="12">
+        <f>AVERAGE(AC23:AC32)</f>
+        <v>61.112000000000002</v>
+      </c>
+      <c r="AD33" s="12">
+        <f>AVERAGE(AD23:AD32)</f>
+        <v>44889.323928779813</v>
+      </c>
+      <c r="AE33" s="12">
+        <f>AVERAGE(AE23:AE32)</f>
+        <v>74.89200000000001</v>
+      </c>
+      <c r="AF33" s="12">
+        <f>AVERAGE(AF23:AF32)</f>
+        <v>61.756000000000007</v>
+      </c>
+    </row>
     <row r="35" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
@@ -3748,13 +6775,13 @@
         <v>66.430000000000007</v>
       </c>
       <c r="AD39">
-        <v>41365.0679248179</v>
+        <v>45529.978999999999</v>
       </c>
       <c r="AE39">
-        <v>81.040000000000006</v>
+        <v>73.63</v>
       </c>
       <c r="AF39">
-        <v>66.83</v>
+        <v>60.72</v>
       </c>
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.3">
@@ -3875,13 +6902,13 @@
         <v>61.22</v>
       </c>
       <c r="I41">
-        <v>38400.353086980802</v>
+        <v>46673.13</v>
       </c>
       <c r="J41">
-        <v>87.3</v>
+        <v>71.83</v>
       </c>
       <c r="K41">
-        <v>71.989999999999995</v>
+        <v>59.23</v>
       </c>
       <c r="L41">
         <v>45875.535614229397</v>
@@ -3938,13 +6965,13 @@
         <v>68.66</v>
       </c>
       <c r="AD41">
-        <v>40740.171004407101</v>
+        <v>49583.976999999999</v>
       </c>
       <c r="AE41">
-        <v>82.29</v>
+        <v>67.61</v>
       </c>
       <c r="AF41">
-        <v>67.849999999999994</v>
+        <v>55.75</v>
       </c>
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.3">
@@ -3970,13 +6997,13 @@
         <v>60.95</v>
       </c>
       <c r="I42">
-        <v>38823.443800182198</v>
+        <v>48836.451000000001</v>
       </c>
       <c r="J42">
-        <v>86.35</v>
+        <v>68.64</v>
       </c>
       <c r="K42">
-        <v>71.2</v>
+        <v>56.6</v>
       </c>
       <c r="L42">
         <v>40939.813507532403</v>
@@ -4015,22 +7042,22 @@
         <v>55.33</v>
       </c>
       <c r="X42">
-        <v>38957.833770408499</v>
+        <v>46002.917000000001</v>
       </c>
       <c r="Y42">
-        <v>86.05</v>
+        <v>72.87</v>
       </c>
       <c r="Z42">
-        <v>70.959999999999994</v>
+        <v>60.09</v>
       </c>
       <c r="AA42">
-        <v>39950.121492631399</v>
+        <v>45988.226000000002</v>
       </c>
       <c r="AB42">
-        <v>83.91</v>
+        <v>72.900000000000006</v>
       </c>
       <c r="AC42">
-        <v>69.2</v>
+        <v>60.11</v>
       </c>
       <c r="AD42">
         <v>41815.742523328001</v>
@@ -4056,13 +7083,13 @@
         <v>63.9</v>
       </c>
       <c r="F43">
-        <v>38479.291592863803</v>
+        <v>52394.385999999999</v>
       </c>
       <c r="G43">
-        <v>87.12</v>
+        <v>63.98</v>
       </c>
       <c r="H43">
-        <v>71.84</v>
+        <v>52.76</v>
       </c>
       <c r="I43">
         <v>43541.725574054297</v>
@@ -4092,13 +7119,13 @@
         <v>53.64</v>
       </c>
       <c r="R43">
-        <v>39546.498612008298</v>
+        <v>49440.864000000001</v>
       </c>
       <c r="S43">
-        <v>84.77</v>
+        <v>67.81</v>
       </c>
       <c r="T43">
-        <v>69.900000000000006</v>
+        <v>55.91</v>
       </c>
       <c r="U43">
         <v>43805.582588596597</v>
@@ -4110,13 +7137,13 @@
         <v>63.11</v>
       </c>
       <c r="X43">
-        <v>35801.339507454599</v>
+        <v>48890.222999999904</v>
       </c>
       <c r="Y43">
-        <v>93.64</v>
+        <v>68.569999999999993</v>
       </c>
       <c r="Z43">
-        <v>77.209999999999994</v>
+        <v>56.54</v>
       </c>
       <c r="AA43">
         <v>41154.835178038797</v>
@@ -4128,13 +7155,13 @@
         <v>67.17</v>
       </c>
       <c r="AD43">
-        <v>38646.219548426197</v>
+        <v>45140.305</v>
       </c>
       <c r="AE43">
-        <v>86.75</v>
+        <v>74.27</v>
       </c>
       <c r="AF43">
-        <v>71.53</v>
+        <v>61.24</v>
       </c>
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.3">
@@ -4214,13 +7241,13 @@
         <v>65.45</v>
       </c>
       <c r="AA44">
-        <v>38275.413771427302</v>
+        <v>53462.512000000002</v>
       </c>
       <c r="AB44">
-        <v>87.59</v>
+        <v>62.71</v>
       </c>
       <c r="AC44">
-        <v>72.22</v>
+        <v>51.71</v>
       </c>
       <c r="AD44">
         <v>46484.620557722301</v>
@@ -4255,13 +7282,13 @@
         <v>61.27</v>
       </c>
       <c r="I45">
-        <v>39033.135315277999</v>
+        <v>44903.133000000002</v>
       </c>
       <c r="J45">
-        <v>85.89</v>
+        <v>74.66</v>
       </c>
       <c r="K45">
-        <v>70.819999999999993</v>
+        <v>61.56</v>
       </c>
       <c r="L45">
         <v>47234.607362390198</v>
@@ -4282,13 +7309,13 @@
         <v>57.34</v>
       </c>
       <c r="R45">
-        <v>40919.875109349101</v>
+        <v>46802.353000000003</v>
       </c>
       <c r="S45">
-        <v>81.93</v>
+        <v>71.63</v>
       </c>
       <c r="T45">
-        <v>67.56</v>
+        <v>59.06</v>
       </c>
       <c r="U45">
         <v>44070.546443995299</v>
@@ -4318,13 +7345,13 @@
         <v>64.02</v>
       </c>
       <c r="AD45">
-        <v>41725.641175869801</v>
+        <v>49558.947</v>
       </c>
       <c r="AE45">
-        <v>80.34</v>
+        <v>67.64</v>
       </c>
       <c r="AF45">
-        <v>66.25</v>
+        <v>55.78</v>
       </c>
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.3">
@@ -4395,13 +7422,13 @@
         <v>64.11</v>
       </c>
       <c r="X46">
-        <v>39318.288325722999</v>
+        <v>46927.656000000003</v>
       </c>
       <c r="Y46">
-        <v>85.26</v>
+        <v>71.44</v>
       </c>
       <c r="Z46">
-        <v>70.31</v>
+        <v>58.91</v>
       </c>
       <c r="AA46">
         <v>47177.752901322703</v>
@@ -4585,31 +7612,156 @@
         <v>65.13</v>
       </c>
       <c r="X48">
-        <v>40228.467789258902</v>
+        <v>47487.203000000001</v>
       </c>
       <c r="Y48">
-        <v>83.33</v>
+        <v>70.599999999999994</v>
       </c>
       <c r="Z48">
-        <v>68.72</v>
+        <v>58.21</v>
       </c>
       <c r="AA48">
-        <v>40183.064536915597</v>
+        <v>48203.182000000001</v>
       </c>
       <c r="AB48">
-        <v>83.43</v>
+        <v>69.55</v>
       </c>
       <c r="AC48">
-        <v>68.790000000000006</v>
+        <v>57.35</v>
       </c>
       <c r="AD48">
-        <v>39118.599595139603</v>
+        <v>44142.241000000002</v>
       </c>
       <c r="AE48">
-        <v>85.7</v>
+        <v>75.94</v>
       </c>
       <c r="AF48">
-        <v>70.67</v>
+        <v>62.62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="B49" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="12">
+        <f>AVERAGE(C39:C48)</f>
+        <v>47680.164899101728</v>
+      </c>
+      <c r="D49" s="12">
+        <f>AVERAGE(D39:D48)</f>
+        <v>70.60799999999999</v>
+      </c>
+      <c r="E49" s="12">
+        <f>AVERAGE(E39:E48)</f>
+        <v>58.224000000000004</v>
+      </c>
+      <c r="F49" s="12">
+        <f>AVERAGE(F39:F48)</f>
+        <v>44837.436550754748</v>
+      </c>
+      <c r="G49" s="12">
+        <f>AVERAGE(G39:G48)</f>
+        <v>75.147000000000006</v>
+      </c>
+      <c r="H49" s="12">
+        <f>AVERAGE(H39:H48)</f>
+        <v>61.966999999999985</v>
+      </c>
+      <c r="I49" s="12">
+        <f>AVERAGE(I39:I48)</f>
+        <v>44339.844799522005</v>
+      </c>
+      <c r="J49" s="12">
+        <f>AVERAGE(J39:J48)</f>
+        <v>75.771000000000001</v>
+      </c>
+      <c r="K49" s="12">
+        <f>AVERAGE(K39:K48)</f>
+        <v>62.481999999999992</v>
+      </c>
+      <c r="L49" s="12">
+        <f>AVERAGE(L39:L48)</f>
+        <v>43439.582744091036</v>
+      </c>
+      <c r="M49" s="12">
+        <f>AVERAGE(M39:M48)</f>
+        <v>77.379000000000005</v>
+      </c>
+      <c r="N49" s="12">
+        <f>AVERAGE(N39:N48)</f>
+        <v>63.804999999999993</v>
+      </c>
+      <c r="O49" s="12">
+        <f>AVERAGE(O39:O48)</f>
+        <v>44402.643189703471</v>
+      </c>
+      <c r="P49" s="12">
+        <f>AVERAGE(P39:P48)</f>
+        <v>76.064999999999998</v>
+      </c>
+      <c r="Q49" s="12">
+        <f>AVERAGE(Q39:Q48)</f>
+        <v>62.722999999999992</v>
+      </c>
+      <c r="R49" s="12">
+        <f>AVERAGE(R39:R48)</f>
+        <v>43768.613270000955</v>
+      </c>
+      <c r="S49" s="12">
+        <f>AVERAGE(S39:S48)</f>
+        <v>76.948999999999998</v>
+      </c>
+      <c r="T49" s="12">
+        <f>AVERAGE(T39:T48)</f>
+        <v>63.45300000000001</v>
+      </c>
+      <c r="U49" s="12">
+        <f>AVERAGE(U39:U48)</f>
+        <v>44896.538901347478</v>
+      </c>
+      <c r="V49" s="12">
+        <f>AVERAGE(V39:V48)</f>
+        <v>75.018000000000001</v>
+      </c>
+      <c r="W49" s="12">
+        <f>AVERAGE(W39:W48)</f>
+        <v>61.861000000000004</v>
+      </c>
+      <c r="X49" s="12">
+        <f>AVERAGE(X39:X48)</f>
+        <v>44642.470277928034</v>
+      </c>
+      <c r="Y49" s="12">
+        <f>AVERAGE(Y39:Y48)</f>
+        <v>75.298000000000016</v>
+      </c>
+      <c r="Z49" s="12">
+        <f>AVERAGE(Z39:Z48)</f>
+        <v>62.090000000000011</v>
+      </c>
+      <c r="AA49" s="12">
+        <f>AVERAGE(AA39:AA48)</f>
+        <v>45015.386576053352</v>
+      </c>
+      <c r="AB49" s="12">
+        <f>AVERAGE(AB39:AB48)</f>
+        <v>74.96899999999998</v>
+      </c>
+      <c r="AC49" s="12">
+        <f>AVERAGE(AC39:AC48)</f>
+        <v>61.818999999999996</v>
+      </c>
+      <c r="AD49" s="12">
+        <f>AVERAGE(AD39:AD48)</f>
+        <v>45005.592412111029</v>
+      </c>
+      <c r="AE49" s="12">
+        <f>AVERAGE(AE39:AE48)</f>
+        <v>74.751000000000005</v>
+      </c>
+      <c r="AF49" s="12">
+        <f>AVERAGE(AF39:AF48)</f>
+        <v>61.64</v>
       </c>
     </row>
     <row r="51" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
@@ -5754,9 +8906,135 @@
         <v>77.67</v>
       </c>
     </row>
+    <row r="65" spans="2:32" x14ac:dyDescent="0.3">
+      <c r="B65" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C65" s="12">
+        <f>AVERAGE(C55:C64)</f>
+        <v>40740.680117002281</v>
+      </c>
+      <c r="D65" s="12">
+        <f>AVERAGE(D55:D64)</f>
+        <v>82.522000000000006</v>
+      </c>
+      <c r="E65" s="12">
+        <f>AVERAGE(E55:E64)</f>
+        <v>68.046999999999997</v>
+      </c>
+      <c r="F65" s="12">
+        <f>AVERAGE(F55:F64)</f>
+        <v>42495.550132819422</v>
+      </c>
+      <c r="G65" s="12">
+        <f>AVERAGE(G55:G64)</f>
+        <v>79.673000000000002</v>
+      </c>
+      <c r="H65" s="12">
+        <f>AVERAGE(H55:H64)</f>
+        <v>65.698000000000008</v>
+      </c>
+      <c r="I65" s="12">
+        <f>AVERAGE(I55:I64)</f>
+        <v>42371.756863898794</v>
+      </c>
+      <c r="J65" s="12">
+        <f>AVERAGE(J55:J64)</f>
+        <v>79.460000000000008</v>
+      </c>
+      <c r="K65" s="12">
+        <f>AVERAGE(K55:K64)</f>
+        <v>65.522999999999996</v>
+      </c>
+      <c r="L65" s="12">
+        <f>AVERAGE(L55:L64)</f>
+        <v>39534.564988198043</v>
+      </c>
+      <c r="M65" s="12">
+        <f>AVERAGE(M55:M64)</f>
+        <v>84.830999999999989</v>
+      </c>
+      <c r="N65" s="12">
+        <f>AVERAGE(N55:N64)</f>
+        <v>69.951999999999998</v>
+      </c>
+      <c r="O65" s="12">
+        <f>AVERAGE(O55:O64)</f>
+        <v>39193.875388758395</v>
+      </c>
+      <c r="P65" s="12">
+        <f>AVERAGE(P55:P64)</f>
+        <v>85.763000000000005</v>
+      </c>
+      <c r="Q65" s="12">
+        <f>AVERAGE(Q55:Q64)</f>
+        <v>70.722000000000008</v>
+      </c>
+      <c r="R65" s="12">
+        <f>AVERAGE(R55:R64)</f>
+        <v>38023.602570881136</v>
+      </c>
+      <c r="S65" s="12">
+        <f>AVERAGE(S55:S64)</f>
+        <v>88.277000000000001</v>
+      </c>
+      <c r="T65" s="12">
+        <f>AVERAGE(T55:T64)</f>
+        <v>72.790999999999983</v>
+      </c>
+      <c r="U65" s="12">
+        <f>AVERAGE(U55:U64)</f>
+        <v>38458.926283995483</v>
+      </c>
+      <c r="V65" s="12">
+        <f>AVERAGE(V55:V64)</f>
+        <v>87.38</v>
+      </c>
+      <c r="W65" s="12">
+        <f>AVERAGE(W55:W64)</f>
+        <v>72.051999999999992</v>
+      </c>
+      <c r="X65" s="12">
+        <f>AVERAGE(X55:X64)</f>
+        <v>39066.91620513508</v>
+      </c>
+      <c r="Y65" s="12">
+        <f>AVERAGE(Y55:Y64)</f>
+        <v>85.991</v>
+      </c>
+      <c r="Z65" s="12">
+        <f>AVERAGE(Z55:Z64)</f>
+        <v>70.908000000000001</v>
+      </c>
+      <c r="AA65" s="12">
+        <f>AVERAGE(AA55:AA64)</f>
+        <v>37502.696591863489</v>
+      </c>
+      <c r="AB65" s="12">
+        <f>AVERAGE(AB55:AB64)</f>
+        <v>89.47799999999998</v>
+      </c>
+      <c r="AC65" s="12">
+        <f>AVERAGE(AC55:AC64)</f>
+        <v>73.783999999999992</v>
+      </c>
+      <c r="AD65" s="12">
+        <f>AVERAGE(AD55:AD64)</f>
+        <v>36552.108284463764</v>
+      </c>
+      <c r="AE65" s="12">
+        <f>AVERAGE(AE55:AE64)</f>
+        <v>91.788000000000011</v>
+      </c>
+      <c r="AF65" s="12">
+        <f>AVERAGE(AF55:AF64)</f>
+        <v>75.69</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Completed Spreadsheet for 48 cities
</commit_message>
<xml_diff>
--- a/Result_sheet.xlsx
+++ b/Result_sheet.xlsx
@@ -13,7 +13,6 @@
   </bookViews>
   <sheets>
     <sheet name="48" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="RMHC_48_100000" localSheetId="0">'48'!$AG$7:$AI$19</definedName>
@@ -2248,6 +2247,785 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1800" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Line Graph showing Efficiency against MST Fitness for 4 different Algorthms for 48 Cities</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Simulated Annealing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>('48'!$D$53,'48'!$G$53,'48'!$J$53,'48'!$M$53,'48'!$P$53,'48'!$S$53,'48'!$V$53,'48'!$Y$53,'48'!$AB$53,'48'!$AE$53)</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('48'!$E$65,'48'!$H$65,'48'!$K$65,'48'!$N$65,'48'!$Q$65,'48'!$T$65,'48'!$W$65,'48'!$Z$65,'48'!$AC$65,'48'!$AF$65)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>68.046999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65.698000000000008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65.522999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69.951999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.722000000000008</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>72.790999999999983</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72.051999999999992</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70.908000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>73.783999999999992</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>75.69</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F9FC-4A0C-9BC2-07336D0E9F20}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Stochastic Hill Climbing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>('48'!$E$49,'48'!$H$49,'48'!$K$49,'48'!$N$49,'48'!$Q$49,'48'!$T$49,'48'!$W$49,'48'!$Z$49,'48'!$AC$49,'48'!$AF$49)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>58.224000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>61.966999999999985</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.481999999999992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63.804999999999993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.722999999999992</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63.45300000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61.861000000000004</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>62.090000000000011</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.818999999999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61.64</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F9FC-4A0C-9BC2-07336D0E9F20}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Random Restart Hill Climbing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>('48'!$E$33,'48'!$H$33,'48'!$K$33,'48'!$N$33,'48'!$Q$33,'48'!$T$33,'48'!$W$33,'48'!$Z$33,'48'!$AC$33,'48'!$AF$33)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>60.501999999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>59.518000000000008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62.744000000000007</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>62.084000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63.092999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63.840000000000011</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61.396999999999991</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>60.71</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61.112000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61.756000000000007</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F9FC-4A0C-9BC2-07336D0E9F20}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Random Mutation Hill Climbing</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:val>
+            <c:numRef>
+              <c:f>('48'!$E$17,'48'!$H$17,'48'!$K$17,'48'!$N$17,'48'!$Q$17,'48'!$T$17,'48'!$W$17,'48'!$Z$17,'48'!$AC$17,'48'!$AF$17)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>57.125000000000014</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58.999000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58.338000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58.311000000000014</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59.491</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55.386000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>58.580999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>59.613999999999997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58.628</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>60.42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F9FC-4A0C-9BC2-07336D0E9F20}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="696527040"/>
+        <c:axId val="787535984"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="696527040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of Iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="787535984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="787535984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Average Efficiency</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="696527040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2289,6 +3067,46 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -3360,6 +4178,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3434,139 +4768,175 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6D18BF3-A044-42B9-8899-35F3FACE844C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_40000" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_20000" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_40000" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_50000" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_90000" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_30000" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_90000" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_30000" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_100000" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_10000" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_10000" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_80000" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_60000" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_20000" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_80000" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_70000" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_60000" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_70000" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_60000" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_20000" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_70000" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_50000" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_10000" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_100000" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_30000" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_40000" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_60000" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_80000" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_70000" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_80000" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_90000" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_100000" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_10000" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_90000" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_20000" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_20000" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_70000" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_50000" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_70000" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_80000" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_60001" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_20000" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_10000" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_60000" connectionId="22" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_10000" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_100000" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_40000" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_100000" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_70000" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_60000" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_30000" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_80000" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_70000" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_50000" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_60000" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_90000" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_90000" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_40000" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RMHC_48_100000" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_30000" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_80000" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SHC_48_60000" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="SA_48_30000" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="RRHC_48_40000" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3868,7 +5238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="Z99" sqref="Z99"/>
     </sheetView>
   </sheetViews>
@@ -5110,123 +6480,123 @@
         <v>12</v>
       </c>
       <c r="C17" s="12">
-        <f>AVERAGE(C7:C16)</f>
+        <f t="shared" ref="C17:AF17" si="0">AVERAGE(C7:C16)</f>
         <v>48604.81815781496</v>
       </c>
       <c r="D17" s="12">
-        <f>AVERAGE(D7:D16)</f>
+        <f t="shared" si="0"/>
         <v>69.277000000000001</v>
       </c>
       <c r="E17" s="12">
-        <f>AVERAGE(E7:E16)</f>
+        <f t="shared" si="0"/>
         <v>57.125000000000014</v>
       </c>
       <c r="F17" s="12">
-        <f>AVERAGE(F7:F16)</f>
+        <f t="shared" si="0"/>
         <v>47359.561565574943</v>
       </c>
       <c r="G17" s="12">
-        <f>AVERAGE(G7:G16)</f>
+        <f t="shared" si="0"/>
         <v>71.546999999999997</v>
       </c>
       <c r="H17" s="12">
-        <f>AVERAGE(H7:H16)</f>
+        <f t="shared" si="0"/>
         <v>58.999000000000002</v>
       </c>
       <c r="I17" s="12">
-        <f>AVERAGE(I7:I16)</f>
+        <f t="shared" si="0"/>
         <v>47692.670660948803</v>
       </c>
       <c r="J17" s="12">
-        <f>AVERAGE(J7:J16)</f>
+        <f t="shared" si="0"/>
         <v>70.747</v>
       </c>
       <c r="K17" s="12">
-        <f>AVERAGE(K7:K16)</f>
+        <f t="shared" si="0"/>
         <v>58.338000000000001</v>
       </c>
       <c r="L17" s="12">
-        <f>AVERAGE(L7:L16)</f>
+        <f t="shared" si="0"/>
         <v>47755.911010290234</v>
       </c>
       <c r="M17" s="12">
-        <f>AVERAGE(M7:M16)</f>
+        <f t="shared" si="0"/>
         <v>70.712999999999994</v>
       </c>
       <c r="N17" s="12">
-        <f>AVERAGE(N7:N16)</f>
+        <f t="shared" si="0"/>
         <v>58.311000000000014</v>
       </c>
       <c r="O17" s="12">
-        <f>AVERAGE(O7:O16)</f>
+        <f t="shared" si="0"/>
         <v>46673.873574000005</v>
       </c>
       <c r="P17" s="12">
-        <f>AVERAGE(P7:P16)</f>
+        <f t="shared" si="0"/>
         <v>72.14500000000001</v>
       </c>
       <c r="Q17" s="12">
-        <f>AVERAGE(Q7:Q16)</f>
+        <f t="shared" si="0"/>
         <v>59.491</v>
       </c>
       <c r="R17" s="12">
-        <f>AVERAGE(R7:R16)</f>
+        <f t="shared" si="0"/>
         <v>50051.412713514968</v>
       </c>
       <c r="S17" s="12">
-        <f>AVERAGE(S7:S16)</f>
+        <f t="shared" si="0"/>
         <v>67.166000000000011</v>
       </c>
       <c r="T17" s="12">
-        <f>AVERAGE(T7:T16)</f>
+        <f t="shared" si="0"/>
         <v>55.386000000000003</v>
       </c>
       <c r="U17" s="12">
-        <f>AVERAGE(U7:U16)</f>
+        <f t="shared" si="0"/>
         <v>47870.426988658422</v>
       </c>
       <c r="V17" s="12">
-        <f>AVERAGE(V7:V16)</f>
+        <f t="shared" si="0"/>
         <v>71.042000000000002</v>
       </c>
       <c r="W17" s="12">
-        <f>AVERAGE(W7:W16)</f>
+        <f t="shared" si="0"/>
         <v>58.580999999999996</v>
       </c>
       <c r="X17" s="12">
-        <f>AVERAGE(X7:X16)</f>
+        <f t="shared" si="0"/>
         <v>46487.498944668492</v>
       </c>
       <c r="Y17" s="12">
-        <f>AVERAGE(Y7:Y16)</f>
+        <f t="shared" si="0"/>
         <v>72.292999999999978</v>
       </c>
       <c r="Z17" s="12">
-        <f>AVERAGE(Z7:Z16)</f>
+        <f t="shared" si="0"/>
         <v>59.613999999999997</v>
       </c>
       <c r="AA17" s="12">
-        <f>AVERAGE(AA7:AA16)</f>
+        <f t="shared" si="0"/>
         <v>47303.808572816313</v>
       </c>
       <c r="AB17" s="12">
-        <f>AVERAGE(AB7:AB16)</f>
+        <f t="shared" si="0"/>
         <v>71.097999999999999</v>
       </c>
       <c r="AC17" s="12">
-        <f>AVERAGE(AC7:AC16)</f>
+        <f t="shared" si="0"/>
         <v>58.628</v>
       </c>
       <c r="AD17" s="12">
-        <f>AVERAGE(AD7:AD16)</f>
+        <f t="shared" si="0"/>
         <v>46179.717035531285</v>
       </c>
       <c r="AE17" s="12">
-        <f>AVERAGE(AE7:AE16)</f>
+        <f t="shared" si="0"/>
         <v>73.269000000000005</v>
       </c>
       <c r="AF17" s="12">
-        <f>AVERAGE(AF7:AF16)</f>
+        <f t="shared" si="0"/>
         <v>60.42</v>
       </c>
     </row>
@@ -6377,123 +7747,123 @@
         <v>12</v>
       </c>
       <c r="C33" s="12">
-        <f>AVERAGE(C23:C32)</f>
+        <f t="shared" ref="C33:AF33" si="1">AVERAGE(C23:C32)</f>
         <v>45949.797477521897</v>
       </c>
       <c r="D33" s="12">
-        <f>AVERAGE(D23:D32)</f>
+        <f t="shared" si="1"/>
         <v>73.371000000000009</v>
       </c>
       <c r="E33" s="12">
-        <f>AVERAGE(E23:E32)</f>
+        <f t="shared" si="1"/>
         <v>60.501999999999995</v>
       </c>
       <c r="F33" s="12">
-        <f>AVERAGE(F23:F32)</f>
+        <f t="shared" si="1"/>
         <v>46675.488346668302</v>
       </c>
       <c r="G33" s="12">
-        <f>AVERAGE(G23:G32)</f>
+        <f t="shared" si="1"/>
         <v>72.174999999999997</v>
       </c>
       <c r="H33" s="12">
-        <f>AVERAGE(H23:H32)</f>
+        <f t="shared" si="1"/>
         <v>59.518000000000008</v>
       </c>
       <c r="I33" s="12">
-        <f>AVERAGE(I23:I32)</f>
+        <f t="shared" si="1"/>
         <v>44212.860590590746</v>
       </c>
       <c r="J33" s="12">
-        <f>AVERAGE(J23:J32)</f>
+        <f t="shared" si="1"/>
         <v>76.09</v>
       </c>
       <c r="K33" s="12">
-        <f>AVERAGE(K23:K32)</f>
+        <f t="shared" si="1"/>
         <v>62.744000000000007</v>
       </c>
       <c r="L33" s="12">
-        <f>AVERAGE(L23:L32)</f>
+        <f t="shared" si="1"/>
         <v>44676.062213810263</v>
       </c>
       <c r="M33" s="12">
-        <f>AVERAGE(M23:M32)</f>
+        <f t="shared" si="1"/>
         <v>75.289999999999992</v>
       </c>
       <c r="N33" s="12">
-        <f>AVERAGE(N23:N32)</f>
+        <f t="shared" si="1"/>
         <v>62.084000000000003</v>
       </c>
       <c r="O33" s="12">
-        <f>AVERAGE(O23:O32)</f>
+        <f t="shared" si="1"/>
         <v>43928.29929568238</v>
       </c>
       <c r="P33" s="12">
-        <f>AVERAGE(P23:P32)</f>
+        <f t="shared" si="1"/>
         <v>76.514999999999986</v>
       </c>
       <c r="Q33" s="12">
-        <f>AVERAGE(Q23:Q32)</f>
+        <f t="shared" si="1"/>
         <v>63.092999999999996</v>
       </c>
       <c r="R33" s="12">
-        <f>AVERAGE(R23:R32)</f>
+        <f t="shared" si="1"/>
         <v>43860.212419729229</v>
       </c>
       <c r="S33" s="12">
-        <f>AVERAGE(S23:S32)</f>
+        <f t="shared" si="1"/>
         <v>77.415999999999997</v>
       </c>
       <c r="T33" s="12">
-        <f>AVERAGE(T23:T32)</f>
+        <f t="shared" si="1"/>
         <v>63.840000000000011</v>
       </c>
       <c r="U33" s="12">
-        <f>AVERAGE(U23:U32)</f>
+        <f t="shared" si="1"/>
         <v>45214.886952463465</v>
       </c>
       <c r="V33" s="12">
-        <f>AVERAGE(V23:V32)</f>
+        <f t="shared" si="1"/>
         <v>74.456999999999994</v>
       </c>
       <c r="W33" s="12">
-        <f>AVERAGE(W23:W32)</f>
+        <f t="shared" si="1"/>
         <v>61.396999999999991</v>
       </c>
       <c r="X33" s="12">
-        <f>AVERAGE(X23:X32)</f>
+        <f t="shared" si="1"/>
         <v>45646.430732534158</v>
       </c>
       <c r="Y33" s="12">
-        <f>AVERAGE(Y23:Y32)</f>
+        <f t="shared" si="1"/>
         <v>73.620999999999995</v>
       </c>
       <c r="Z33" s="12">
-        <f>AVERAGE(Z23:Z32)</f>
+        <f t="shared" si="1"/>
         <v>60.71</v>
       </c>
       <c r="AA33" s="12">
-        <f>AVERAGE(AA23:AA32)</f>
+        <f t="shared" si="1"/>
         <v>45314.593443100501</v>
       </c>
       <c r="AB33" s="12">
-        <f>AVERAGE(AB23:AB32)</f>
+        <f t="shared" si="1"/>
         <v>74.108999999999995</v>
       </c>
       <c r="AC33" s="12">
-        <f>AVERAGE(AC23:AC32)</f>
+        <f t="shared" si="1"/>
         <v>61.112000000000002</v>
       </c>
       <c r="AD33" s="12">
-        <f>AVERAGE(AD23:AD32)</f>
+        <f t="shared" si="1"/>
         <v>44889.323928779813</v>
       </c>
       <c r="AE33" s="12">
-        <f>AVERAGE(AE23:AE32)</f>
+        <f t="shared" si="1"/>
         <v>74.89200000000001</v>
       </c>
       <c r="AF33" s="12">
-        <f>AVERAGE(AF23:AF32)</f>
+        <f t="shared" si="1"/>
         <v>61.756000000000007</v>
       </c>
     </row>
@@ -7644,123 +9014,123 @@
         <v>12</v>
       </c>
       <c r="C49" s="12">
-        <f>AVERAGE(C39:C48)</f>
+        <f t="shared" ref="C49:AF49" si="2">AVERAGE(C39:C48)</f>
         <v>47680.164899101728</v>
       </c>
       <c r="D49" s="12">
-        <f>AVERAGE(D39:D48)</f>
+        <f t="shared" si="2"/>
         <v>70.60799999999999</v>
       </c>
       <c r="E49" s="12">
-        <f>AVERAGE(E39:E48)</f>
+        <f t="shared" si="2"/>
         <v>58.224000000000004</v>
       </c>
       <c r="F49" s="12">
-        <f>AVERAGE(F39:F48)</f>
+        <f t="shared" si="2"/>
         <v>44837.436550754748</v>
       </c>
       <c r="G49" s="12">
-        <f>AVERAGE(G39:G48)</f>
+        <f t="shared" si="2"/>
         <v>75.147000000000006</v>
       </c>
       <c r="H49" s="12">
-        <f>AVERAGE(H39:H48)</f>
+        <f t="shared" si="2"/>
         <v>61.966999999999985</v>
       </c>
       <c r="I49" s="12">
-        <f>AVERAGE(I39:I48)</f>
+        <f t="shared" si="2"/>
         <v>44339.844799522005</v>
       </c>
       <c r="J49" s="12">
-        <f>AVERAGE(J39:J48)</f>
+        <f t="shared" si="2"/>
         <v>75.771000000000001</v>
       </c>
       <c r="K49" s="12">
-        <f>AVERAGE(K39:K48)</f>
+        <f t="shared" si="2"/>
         <v>62.481999999999992</v>
       </c>
       <c r="L49" s="12">
-        <f>AVERAGE(L39:L48)</f>
+        <f t="shared" si="2"/>
         <v>43439.582744091036</v>
       </c>
       <c r="M49" s="12">
-        <f>AVERAGE(M39:M48)</f>
+        <f t="shared" si="2"/>
         <v>77.379000000000005</v>
       </c>
       <c r="N49" s="12">
-        <f>AVERAGE(N39:N48)</f>
+        <f t="shared" si="2"/>
         <v>63.804999999999993</v>
       </c>
       <c r="O49" s="12">
-        <f>AVERAGE(O39:O48)</f>
+        <f t="shared" si="2"/>
         <v>44402.643189703471</v>
       </c>
       <c r="P49" s="12">
-        <f>AVERAGE(P39:P48)</f>
+        <f t="shared" si="2"/>
         <v>76.064999999999998</v>
       </c>
       <c r="Q49" s="12">
-        <f>AVERAGE(Q39:Q48)</f>
+        <f t="shared" si="2"/>
         <v>62.722999999999992</v>
       </c>
       <c r="R49" s="12">
-        <f>AVERAGE(R39:R48)</f>
+        <f t="shared" si="2"/>
         <v>43768.613270000955</v>
       </c>
       <c r="S49" s="12">
-        <f>AVERAGE(S39:S48)</f>
+        <f t="shared" si="2"/>
         <v>76.948999999999998</v>
       </c>
       <c r="T49" s="12">
-        <f>AVERAGE(T39:T48)</f>
+        <f t="shared" si="2"/>
         <v>63.45300000000001</v>
       </c>
       <c r="U49" s="12">
-        <f>AVERAGE(U39:U48)</f>
+        <f t="shared" si="2"/>
         <v>44896.538901347478</v>
       </c>
       <c r="V49" s="12">
-        <f>AVERAGE(V39:V48)</f>
+        <f t="shared" si="2"/>
         <v>75.018000000000001</v>
       </c>
       <c r="W49" s="12">
-        <f>AVERAGE(W39:W48)</f>
+        <f t="shared" si="2"/>
         <v>61.861000000000004</v>
       </c>
       <c r="X49" s="12">
-        <f>AVERAGE(X39:X48)</f>
+        <f t="shared" si="2"/>
         <v>44642.470277928034</v>
       </c>
       <c r="Y49" s="12">
-        <f>AVERAGE(Y39:Y48)</f>
+        <f t="shared" si="2"/>
         <v>75.298000000000016</v>
       </c>
       <c r="Z49" s="12">
-        <f>AVERAGE(Z39:Z48)</f>
+        <f t="shared" si="2"/>
         <v>62.090000000000011</v>
       </c>
       <c r="AA49" s="12">
-        <f>AVERAGE(AA39:AA48)</f>
+        <f t="shared" si="2"/>
         <v>45015.386576053352</v>
       </c>
       <c r="AB49" s="12">
-        <f>AVERAGE(AB39:AB48)</f>
+        <f t="shared" si="2"/>
         <v>74.96899999999998</v>
       </c>
       <c r="AC49" s="12">
-        <f>AVERAGE(AC39:AC48)</f>
+        <f t="shared" si="2"/>
         <v>61.818999999999996</v>
       </c>
       <c r="AD49" s="12">
-        <f>AVERAGE(AD39:AD48)</f>
+        <f t="shared" si="2"/>
         <v>45005.592412111029</v>
       </c>
       <c r="AE49" s="12">
-        <f>AVERAGE(AE39:AE48)</f>
+        <f t="shared" si="2"/>
         <v>74.751000000000005</v>
       </c>
       <c r="AF49" s="12">
-        <f>AVERAGE(AF39:AF48)</f>
+        <f t="shared" si="2"/>
         <v>61.64</v>
       </c>
     </row>
@@ -8911,123 +10281,123 @@
         <v>12</v>
       </c>
       <c r="C65" s="12">
-        <f>AVERAGE(C55:C64)</f>
+        <f t="shared" ref="C65:AF65" si="3">AVERAGE(C55:C64)</f>
         <v>40740.680117002281</v>
       </c>
       <c r="D65" s="12">
-        <f>AVERAGE(D55:D64)</f>
+        <f t="shared" si="3"/>
         <v>82.522000000000006</v>
       </c>
       <c r="E65" s="12">
-        <f>AVERAGE(E55:E64)</f>
+        <f t="shared" si="3"/>
         <v>68.046999999999997</v>
       </c>
       <c r="F65" s="12">
-        <f>AVERAGE(F55:F64)</f>
+        <f t="shared" si="3"/>
         <v>42495.550132819422</v>
       </c>
       <c r="G65" s="12">
-        <f>AVERAGE(G55:G64)</f>
+        <f t="shared" si="3"/>
         <v>79.673000000000002</v>
       </c>
       <c r="H65" s="12">
-        <f>AVERAGE(H55:H64)</f>
+        <f t="shared" si="3"/>
         <v>65.698000000000008</v>
       </c>
       <c r="I65" s="12">
-        <f>AVERAGE(I55:I64)</f>
+        <f t="shared" si="3"/>
         <v>42371.756863898794</v>
       </c>
       <c r="J65" s="12">
-        <f>AVERAGE(J55:J64)</f>
+        <f t="shared" si="3"/>
         <v>79.460000000000008</v>
       </c>
       <c r="K65" s="12">
-        <f>AVERAGE(K55:K64)</f>
+        <f t="shared" si="3"/>
         <v>65.522999999999996</v>
       </c>
       <c r="L65" s="12">
-        <f>AVERAGE(L55:L64)</f>
+        <f t="shared" si="3"/>
         <v>39534.564988198043</v>
       </c>
       <c r="M65" s="12">
-        <f>AVERAGE(M55:M64)</f>
+        <f t="shared" si="3"/>
         <v>84.830999999999989</v>
       </c>
       <c r="N65" s="12">
-        <f>AVERAGE(N55:N64)</f>
+        <f t="shared" si="3"/>
         <v>69.951999999999998</v>
       </c>
       <c r="O65" s="12">
-        <f>AVERAGE(O55:O64)</f>
+        <f t="shared" si="3"/>
         <v>39193.875388758395</v>
       </c>
       <c r="P65" s="12">
-        <f>AVERAGE(P55:P64)</f>
+        <f t="shared" si="3"/>
         <v>85.763000000000005</v>
       </c>
       <c r="Q65" s="12">
-        <f>AVERAGE(Q55:Q64)</f>
+        <f t="shared" si="3"/>
         <v>70.722000000000008</v>
       </c>
       <c r="R65" s="12">
-        <f>AVERAGE(R55:R64)</f>
+        <f t="shared" si="3"/>
         <v>38023.602570881136</v>
       </c>
       <c r="S65" s="12">
-        <f>AVERAGE(S55:S64)</f>
+        <f t="shared" si="3"/>
         <v>88.277000000000001</v>
       </c>
       <c r="T65" s="12">
-        <f>AVERAGE(T55:T64)</f>
+        <f t="shared" si="3"/>
         <v>72.790999999999983</v>
       </c>
       <c r="U65" s="12">
-        <f>AVERAGE(U55:U64)</f>
+        <f t="shared" si="3"/>
         <v>38458.926283995483</v>
       </c>
       <c r="V65" s="12">
-        <f>AVERAGE(V55:V64)</f>
+        <f t="shared" si="3"/>
         <v>87.38</v>
       </c>
       <c r="W65" s="12">
-        <f>AVERAGE(W55:W64)</f>
+        <f t="shared" si="3"/>
         <v>72.051999999999992</v>
       </c>
       <c r="X65" s="12">
-        <f>AVERAGE(X55:X64)</f>
+        <f t="shared" si="3"/>
         <v>39066.91620513508</v>
       </c>
       <c r="Y65" s="12">
-        <f>AVERAGE(Y55:Y64)</f>
+        <f t="shared" si="3"/>
         <v>85.991</v>
       </c>
       <c r="Z65" s="12">
-        <f>AVERAGE(Z55:Z64)</f>
+        <f t="shared" si="3"/>
         <v>70.908000000000001</v>
       </c>
       <c r="AA65" s="12">
-        <f>AVERAGE(AA55:AA64)</f>
+        <f t="shared" si="3"/>
         <v>37502.696591863489</v>
       </c>
       <c r="AB65" s="12">
-        <f>AVERAGE(AB55:AB64)</f>
+        <f t="shared" si="3"/>
         <v>89.47799999999998</v>
       </c>
       <c r="AC65" s="12">
-        <f>AVERAGE(AC55:AC64)</f>
+        <f t="shared" si="3"/>
         <v>73.783999999999992</v>
       </c>
       <c r="AD65" s="12">
-        <f>AVERAGE(AD55:AD64)</f>
+        <f t="shared" si="3"/>
         <v>36552.108284463764</v>
       </c>
       <c r="AE65" s="12">
-        <f>AVERAGE(AE55:AE64)</f>
+        <f t="shared" si="3"/>
         <v>91.788000000000011</v>
       </c>
       <c r="AF65" s="12">
-        <f>AVERAGE(AF55:AF64)</f>
+        <f t="shared" si="3"/>
         <v>75.69</v>
       </c>
     </row>
@@ -9036,22 +10406,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="6" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>